<commit_message>
Update results of 001 -> 004
</commit_message>
<xml_diff>
--- a/20160405 - 001/running_logs/logs.xlsx
+++ b/20160405 - 001/running_logs/logs.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="39">
   <si>
     <t>Time</t>
   </si>
@@ -89,6 +89,48 @@
   </si>
   <si>
     <t>20160405_161207</t>
+  </si>
+  <si>
+    <t>20160406_104313</t>
+  </si>
+  <si>
+    <t>trim "space" and ",", remove multiple spaces, convert to lower, convert unicode to ascii</t>
+  </si>
+  <si>
+    <t>2 layers: [100-Sigmoid, 3-Softmax], learning_rate: 0.01, learning_rule: adagrad, n_iterator: 1000</t>
+  </si>
+  <si>
+    <t>20160406_110216</t>
+  </si>
+  <si>
+    <t>20160406_112141</t>
+  </si>
+  <si>
+    <t>20160406_114200</t>
+  </si>
+  <si>
+    <t>20160406_120232</t>
+  </si>
+  <si>
+    <t>20160406_133424</t>
+  </si>
+  <si>
+    <t>remove multiple spaces, convert unicode to ascii, trim "space" and ",", convert to lower</t>
+  </si>
+  <si>
+    <t>2 layers: [100-Sigmoid, 3-Softmax], learning_rate: 0.01, learning_rule: adagrad, n_iterator: 2000</t>
+  </si>
+  <si>
+    <t>20160406_141728</t>
+  </si>
+  <si>
+    <t>20160406_150152</t>
+  </si>
+  <si>
+    <t>20160406_153110</t>
+  </si>
+  <si>
+    <t>20160406_155852</t>
   </si>
 </sst>
 </file>
@@ -420,7 +462,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -775,6 +817,326 @@
         <v>0.0434782608695652</v>
       </c>
     </row>
+    <row r="12" spans="1:10">
+      <c r="A12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12">
+        <v>1142.736</v>
+      </c>
+      <c r="C12" t="s">
+        <v>26</v>
+      </c>
+      <c r="D12" t="s">
+        <v>11</v>
+      </c>
+      <c r="E12" t="s">
+        <v>12</v>
+      </c>
+      <c r="F12" t="s">
+        <v>27</v>
+      </c>
+      <c r="G12">
+        <v>0.999333333333333</v>
+      </c>
+      <c r="H12">
+        <v>0.920792079207921</v>
+      </c>
+      <c r="I12" t="s">
+        <v>14</v>
+      </c>
+      <c r="J12">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
+      <c r="A13" t="s">
+        <v>28</v>
+      </c>
+      <c r="B13">
+        <v>1164.935</v>
+      </c>
+      <c r="C13" t="s">
+        <v>26</v>
+      </c>
+      <c r="D13" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13" t="s">
+        <v>12</v>
+      </c>
+      <c r="F13" t="s">
+        <v>27</v>
+      </c>
+      <c r="G13">
+        <v>1</v>
+      </c>
+      <c r="H13">
+        <v>0.894389438943894</v>
+      </c>
+      <c r="I13" t="s">
+        <v>14</v>
+      </c>
+      <c r="J13">
+        <v>0.0447761194029851</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
+      <c r="A14" t="s">
+        <v>29</v>
+      </c>
+      <c r="B14">
+        <v>1218.655</v>
+      </c>
+      <c r="C14" t="s">
+        <v>26</v>
+      </c>
+      <c r="D14" t="s">
+        <v>11</v>
+      </c>
+      <c r="E14" t="s">
+        <v>12</v>
+      </c>
+      <c r="F14" t="s">
+        <v>27</v>
+      </c>
+      <c r="G14">
+        <v>0.998666666666667</v>
+      </c>
+      <c r="H14">
+        <v>0.937293729372937</v>
+      </c>
+      <c r="I14" t="s">
+        <v>14</v>
+      </c>
+      <c r="J14">
+        <v>0.0375</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
+      <c r="A15" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15">
+        <v>1232.143</v>
+      </c>
+      <c r="C15" t="s">
+        <v>26</v>
+      </c>
+      <c r="D15" t="s">
+        <v>11</v>
+      </c>
+      <c r="E15" t="s">
+        <v>12</v>
+      </c>
+      <c r="F15" t="s">
+        <v>27</v>
+      </c>
+      <c r="G15">
+        <v>1</v>
+      </c>
+      <c r="H15">
+        <v>0.884488448844885</v>
+      </c>
+      <c r="I15" t="s">
+        <v>14</v>
+      </c>
+      <c r="J15">
+        <v>0.0625</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
+      <c r="A16" t="s">
+        <v>31</v>
+      </c>
+      <c r="B16">
+        <v>1322.821</v>
+      </c>
+      <c r="C16" t="s">
+        <v>26</v>
+      </c>
+      <c r="D16" t="s">
+        <v>11</v>
+      </c>
+      <c r="E16" t="s">
+        <v>12</v>
+      </c>
+      <c r="F16" t="s">
+        <v>27</v>
+      </c>
+      <c r="G16">
+        <v>1</v>
+      </c>
+      <c r="H16">
+        <v>0.874587458745875</v>
+      </c>
+      <c r="I16" t="s">
+        <v>14</v>
+      </c>
+      <c r="J16">
+        <v>0.0491803278688525</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10">
+      <c r="A17" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17">
+        <v>2583.971</v>
+      </c>
+      <c r="C17" t="s">
+        <v>33</v>
+      </c>
+      <c r="D17" t="s">
+        <v>11</v>
+      </c>
+      <c r="E17" t="s">
+        <v>12</v>
+      </c>
+      <c r="F17" t="s">
+        <v>34</v>
+      </c>
+      <c r="G17">
+        <v>0.999333333333333</v>
+      </c>
+      <c r="H17">
+        <v>0.900990099009901</v>
+      </c>
+      <c r="I17" t="s">
+        <v>14</v>
+      </c>
+      <c r="J17">
+        <v>0.0579710144927536</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10">
+      <c r="A18" t="s">
+        <v>35</v>
+      </c>
+      <c r="B18">
+        <v>2664.168</v>
+      </c>
+      <c r="C18" t="s">
+        <v>33</v>
+      </c>
+      <c r="D18" t="s">
+        <v>11</v>
+      </c>
+      <c r="E18" t="s">
+        <v>12</v>
+      </c>
+      <c r="F18" t="s">
+        <v>34</v>
+      </c>
+      <c r="G18">
+        <v>1</v>
+      </c>
+      <c r="H18">
+        <v>0.897689768976898</v>
+      </c>
+      <c r="I18" t="s">
+        <v>14</v>
+      </c>
+      <c r="J18">
+        <v>0.0588235294117647</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
+      <c r="A19" t="s">
+        <v>36</v>
+      </c>
+      <c r="B19">
+        <v>1758.119</v>
+      </c>
+      <c r="C19" t="s">
+        <v>33</v>
+      </c>
+      <c r="D19" t="s">
+        <v>11</v>
+      </c>
+      <c r="E19" t="s">
+        <v>12</v>
+      </c>
+      <c r="F19" t="s">
+        <v>34</v>
+      </c>
+      <c r="G19">
+        <v>0.999333333333333</v>
+      </c>
+      <c r="H19">
+        <v>0.910891089108911</v>
+      </c>
+      <c r="I19" t="s">
+        <v>14</v>
+      </c>
+      <c r="J19">
+        <v>0.0416666666666667</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10">
+      <c r="A20" t="s">
+        <v>37</v>
+      </c>
+      <c r="B20">
+        <v>1661.828</v>
+      </c>
+      <c r="C20" t="s">
+        <v>33</v>
+      </c>
+      <c r="D20" t="s">
+        <v>11</v>
+      </c>
+      <c r="E20" t="s">
+        <v>12</v>
+      </c>
+      <c r="F20" t="s">
+        <v>34</v>
+      </c>
+      <c r="G20">
+        <v>0.999333333333333</v>
+      </c>
+      <c r="H20">
+        <v>0.900990099009901</v>
+      </c>
+      <c r="I20" t="s">
+        <v>14</v>
+      </c>
+      <c r="J20">
+        <v>0.0434782608695652</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10">
+      <c r="A21" t="s">
+        <v>38</v>
+      </c>
+      <c r="B21">
+        <v>1516.028</v>
+      </c>
+      <c r="C21" t="s">
+        <v>33</v>
+      </c>
+      <c r="D21" t="s">
+        <v>11</v>
+      </c>
+      <c r="E21" t="s">
+        <v>12</v>
+      </c>
+      <c r="F21" t="s">
+        <v>34</v>
+      </c>
+      <c r="G21">
+        <v>1</v>
+      </c>
+      <c r="H21">
+        <v>0.874587458745875</v>
+      </c>
+      <c r="I21" t="s">
+        <v>14</v>
+      </c>
+      <c r="J21">
+        <v>0.0819672131147541</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>